<commit_message>
Add data for TNRS guide
</commit_message>
<xml_diff>
--- a/LAB/lab02/_docs/Datos_TNRS.xlsx
+++ b/LAB/lab02/_docs/Datos_TNRS.xlsx
@@ -792,9 +792,6 @@
     <t>Ricinus</t>
   </si>
   <si>
-    <t>communis</t>
-  </si>
-  <si>
     <t>Universidad de Antioquia</t>
   </si>
   <si>
@@ -1171,6 +1168,9 @@
   </si>
   <si>
     <t>cumensis</t>
+  </si>
+  <si>
+    <t>comunis</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1537,7 @@
   <dimension ref="A1:AW35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AL28" sqref="AL28"/>
+      <selection activeCell="AL35" sqref="AL35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1747,7 +1747,7 @@
         <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J2" t="s">
         <v>67</v>
@@ -1765,7 +1765,7 @@
         <v>69</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P2" t="s">
         <v>53</v>
@@ -1783,7 +1783,7 @@
         <v>70</v>
       </c>
       <c r="V2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="W2" t="s">
         <v>71</v>
@@ -1810,7 +1810,7 @@
         <v>73</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AF2" t="s">
         <v>74</v>
@@ -1878,7 +1878,7 @@
         <v>49</v>
       </c>
       <c r="I3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J3" t="s">
         <v>85</v>
@@ -1896,7 +1896,7 @@
         <v>69</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P3" t="s">
         <v>53</v>
@@ -1914,7 +1914,7 @@
         <v>70</v>
       </c>
       <c r="V3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W3" t="s">
         <v>95</v>
@@ -1941,13 +1941,13 @@
         <v>86</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF3" t="s">
         <v>74</v>
       </c>
       <c r="AG3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AI3" t="s">
         <v>67</v>
@@ -2009,7 +2009,7 @@
         <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J4" t="s">
         <v>97</v>
@@ -2027,7 +2027,7 @@
         <v>69</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P4" t="s">
         <v>53</v>
@@ -2072,7 +2072,7 @@
         <v>86</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF4" t="s">
         <v>74</v>
@@ -2137,7 +2137,7 @@
         <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J5" t="s">
         <v>106</v>
@@ -2155,7 +2155,7 @@
         <v>69</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P5" t="s">
         <v>53</v>
@@ -2173,7 +2173,7 @@
         <v>70</v>
       </c>
       <c r="V5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="W5" t="s">
         <v>107</v>
@@ -2200,19 +2200,19 @@
         <v>86</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF5" t="s">
         <v>74</v>
       </c>
       <c r="AG5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AI5" t="s">
         <v>106</v>
       </c>
       <c r="AL5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AM5" t="s">
         <v>56</v>
@@ -2271,7 +2271,7 @@
         <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J6" t="s">
         <v>97</v>
@@ -2289,7 +2289,7 @@
         <v>69</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P6" t="s">
         <v>53</v>
@@ -2328,7 +2328,7 @@
         <v>73</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF6" t="s">
         <v>74</v>
@@ -2343,7 +2343,7 @@
         <v>2009</v>
       </c>
       <c r="AL6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AM6" t="s">
         <v>56</v>
@@ -2396,7 +2396,7 @@
         <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J7" t="s">
         <v>67</v>
@@ -2453,7 +2453,7 @@
         <v>73</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF7" t="s">
         <v>74</v>
@@ -2468,7 +2468,7 @@
         <v>124</v>
       </c>
       <c r="AL7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AM7" t="s">
         <v>56</v>
@@ -2521,7 +2521,7 @@
         <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J8" t="s">
         <v>97</v>
@@ -2578,7 +2578,7 @@
         <v>73</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF8" t="s">
         <v>74</v>
@@ -2587,7 +2587,7 @@
         <v>115</v>
       </c>
       <c r="AL8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AM8" t="s">
         <v>56</v>
@@ -2640,7 +2640,7 @@
         <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J9" t="s">
         <v>67</v>
@@ -2700,7 +2700,7 @@
         <v>73</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF9" t="s">
         <v>74</v>
@@ -2765,7 +2765,7 @@
         <v>49</v>
       </c>
       <c r="I10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J10" t="s">
         <v>97</v>
@@ -2783,7 +2783,7 @@
         <v>69</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P10" t="s">
         <v>53</v>
@@ -2828,7 +2828,7 @@
         <v>86</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF10" t="s">
         <v>74</v>
@@ -2893,7 +2893,7 @@
         <v>49</v>
       </c>
       <c r="I11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J11" t="s">
         <v>67</v>
@@ -2911,7 +2911,7 @@
         <v>69</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P11" t="s">
         <v>53</v>
@@ -2950,7 +2950,7 @@
         <v>73</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AF11" t="s">
         <v>74</v>
@@ -3015,7 +3015,7 @@
         <v>49</v>
       </c>
       <c r="I12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J12" t="s">
         <v>150</v>
@@ -3033,7 +3033,7 @@
         <v>69</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P12" t="s">
         <v>53</v>
@@ -3078,13 +3078,13 @@
         <v>73</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AF12" t="s">
         <v>74</v>
       </c>
       <c r="AG12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AI12" t="s">
         <v>67</v>
@@ -3096,7 +3096,7 @@
         <v>154</v>
       </c>
       <c r="AL12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AM12" t="s">
         <v>56</v>
@@ -3149,7 +3149,7 @@
         <v>49</v>
       </c>
       <c r="I13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="J13" t="s">
         <v>159</v>
@@ -3167,7 +3167,7 @@
         <v>69</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P13" t="s">
         <v>53</v>
@@ -3209,13 +3209,13 @@
         <v>73</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AF13" t="s">
         <v>74</v>
       </c>
       <c r="AG13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AH13" t="s">
         <v>163</v>
@@ -3286,7 +3286,7 @@
         <v>49</v>
       </c>
       <c r="I14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="J14" t="s">
         <v>150</v>
@@ -3304,7 +3304,7 @@
         <v>69</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P14" t="s">
         <v>53</v>
@@ -3349,13 +3349,13 @@
         <v>73</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AF14" t="s">
         <v>74</v>
       </c>
       <c r="AG14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AI14" t="s">
         <v>67</v>
@@ -3367,7 +3367,7 @@
         <v>168</v>
       </c>
       <c r="AL14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AM14" t="s">
         <v>56</v>
@@ -3420,7 +3420,7 @@
         <v>49</v>
       </c>
       <c r="I15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J15" t="s">
         <v>159</v>
@@ -3438,7 +3438,7 @@
         <v>69</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P15" t="s">
         <v>53</v>
@@ -3483,13 +3483,13 @@
         <v>73</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="AF15" t="s">
         <v>74</v>
       </c>
       <c r="AG15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AI15" t="s">
         <v>67</v>
@@ -3548,7 +3548,7 @@
         <v>49</v>
       </c>
       <c r="I16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J16" t="s">
         <v>175</v>
@@ -3566,7 +3566,7 @@
         <v>69</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P16" t="s">
         <v>53</v>
@@ -3611,13 +3611,13 @@
         <v>178</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF16" t="s">
         <v>74</v>
       </c>
       <c r="AG16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AI16" t="s">
         <v>67</v>
@@ -3626,7 +3626,7 @@
         <v>1970</v>
       </c>
       <c r="AL16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AM16" t="s">
         <v>56</v>
@@ -3682,7 +3682,7 @@
         <v>49</v>
       </c>
       <c r="I17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="J17" t="s">
         <v>159</v>
@@ -3700,7 +3700,7 @@
         <v>69</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P17" t="s">
         <v>53</v>
@@ -3745,13 +3745,13 @@
         <v>73</v>
       </c>
       <c r="AE17" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="AF17" t="s">
         <v>74</v>
       </c>
       <c r="AG17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AI17" t="s">
         <v>184</v>
@@ -3816,7 +3816,7 @@
         <v>49</v>
       </c>
       <c r="I18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="J18" t="s">
         <v>97</v>
@@ -3834,7 +3834,7 @@
         <v>69</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P18" t="s">
         <v>53</v>
@@ -3879,7 +3879,7 @@
         <v>86</v>
       </c>
       <c r="AE18" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF18" t="s">
         <v>74</v>
@@ -3944,7 +3944,7 @@
         <v>49</v>
       </c>
       <c r="I19" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J19" t="s">
         <v>97</v>
@@ -3962,7 +3962,7 @@
         <v>69</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P19" t="s">
         <v>53</v>
@@ -4007,19 +4007,19 @@
         <v>86</v>
       </c>
       <c r="AE19" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AF19" t="s">
         <v>74</v>
       </c>
       <c r="AG19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AH19" t="s">
         <v>200</v>
       </c>
       <c r="AL19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AM19" t="s">
         <v>56</v>
@@ -4037,7 +4037,7 @@
         <v>201</v>
       </c>
       <c r="AR19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AS19" t="s">
         <v>202</v>
@@ -4075,7 +4075,7 @@
         <v>49</v>
       </c>
       <c r="I20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J20" t="s">
         <v>97</v>
@@ -4093,7 +4093,7 @@
         <v>69</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P20" t="s">
         <v>53</v>
@@ -4138,13 +4138,13 @@
         <v>86</v>
       </c>
       <c r="AE20" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AF20" t="s">
         <v>74</v>
       </c>
       <c r="AG20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AH20" t="s">
         <v>200</v>
@@ -4206,7 +4206,7 @@
         <v>49</v>
       </c>
       <c r="I21" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J21" t="s">
         <v>97</v>
@@ -4224,7 +4224,7 @@
         <v>69</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P21" t="s">
         <v>53</v>
@@ -4269,7 +4269,7 @@
         <v>86</v>
       </c>
       <c r="AE21" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF21" t="s">
         <v>74</v>
@@ -4284,7 +4284,7 @@
         <v>1971</v>
       </c>
       <c r="AL21" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AM21" t="s">
         <v>56</v>
@@ -4340,7 +4340,7 @@
         <v>49</v>
       </c>
       <c r="I22" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J22" t="s">
         <v>97</v>
@@ -4358,7 +4358,7 @@
         <v>69</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P22" t="s">
         <v>53</v>
@@ -4403,7 +4403,7 @@
         <v>86</v>
       </c>
       <c r="AE22" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF22" t="s">
         <v>74</v>
@@ -4418,7 +4418,7 @@
         <v>1971</v>
       </c>
       <c r="AL22" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AM22" t="s">
         <v>56</v>
@@ -4474,7 +4474,7 @@
         <v>49</v>
       </c>
       <c r="I23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J23" t="s">
         <v>97</v>
@@ -4492,7 +4492,7 @@
         <v>69</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P23" t="s">
         <v>53</v>
@@ -4537,7 +4537,7 @@
         <v>86</v>
       </c>
       <c r="AE23" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AF23" t="s">
         <v>74</v>
@@ -4602,7 +4602,7 @@
         <v>49</v>
       </c>
       <c r="I24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J24" t="s">
         <v>97</v>
@@ -4620,7 +4620,7 @@
         <v>69</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P24" t="s">
         <v>53</v>
@@ -4665,13 +4665,13 @@
         <v>86</v>
       </c>
       <c r="AE24" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AF24" t="s">
         <v>74</v>
       </c>
       <c r="AG24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AH24" t="s">
         <v>200</v>
@@ -4733,7 +4733,7 @@
         <v>49</v>
       </c>
       <c r="I25" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J25" t="s">
         <v>220</v>
@@ -4751,7 +4751,7 @@
         <v>69</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P25" t="s">
         <v>53</v>
@@ -4790,7 +4790,7 @@
         <v>224</v>
       </c>
       <c r="AE25" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF25" t="s">
         <v>74</v>
@@ -4805,7 +4805,7 @@
         <v>2009</v>
       </c>
       <c r="AL25" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AM25" t="s">
         <v>56</v>
@@ -4826,7 +4826,7 @@
         <v>228</v>
       </c>
       <c r="AS25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AU25" t="s">
         <v>57</v>
@@ -4861,7 +4861,7 @@
         <v>49</v>
       </c>
       <c r="I26" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J26" t="s">
         <v>220</v>
@@ -4879,7 +4879,7 @@
         <v>69</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P26" t="s">
         <v>53</v>
@@ -4918,7 +4918,7 @@
         <v>224</v>
       </c>
       <c r="AE26" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF26" t="s">
         <v>74</v>
@@ -4983,7 +4983,7 @@
         <v>49</v>
       </c>
       <c r="I27" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J27" t="s">
         <v>220</v>
@@ -5001,7 +5001,7 @@
         <v>69</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P27" t="s">
         <v>53</v>
@@ -5040,7 +5040,7 @@
         <v>86</v>
       </c>
       <c r="AE27" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF27" t="s">
         <v>74</v>
@@ -5111,7 +5111,7 @@
         <v>49</v>
       </c>
       <c r="I28" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J28" t="s">
         <v>220</v>
@@ -5129,7 +5129,7 @@
         <v>69</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P28" t="s">
         <v>53</v>
@@ -5168,7 +5168,7 @@
         <v>224</v>
       </c>
       <c r="AE28" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF28" t="s">
         <v>74</v>
@@ -5236,7 +5236,7 @@
         <v>49</v>
       </c>
       <c r="I29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J29" t="s">
         <v>220</v>
@@ -5254,7 +5254,7 @@
         <v>69</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P29" t="s">
         <v>53</v>
@@ -5293,7 +5293,7 @@
         <v>86</v>
       </c>
       <c r="AE29" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF29" t="s">
         <v>74</v>
@@ -5308,7 +5308,7 @@
         <v>1970</v>
       </c>
       <c r="AL29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AM29" t="s">
         <v>56</v>
@@ -5329,7 +5329,7 @@
         <v>256</v>
       </c>
       <c r="AS29" t="s">
-        <v>257</v>
+        <v>383</v>
       </c>
       <c r="AU29" t="s">
         <v>57</v>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="30" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B30" t="s">
         <v>50</v>
@@ -5364,7 +5364,7 @@
         <v>49</v>
       </c>
       <c r="I30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J30" t="s">
         <v>220</v>
@@ -5382,7 +5382,7 @@
         <v>69</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P30" t="s">
         <v>53</v>
@@ -5403,7 +5403,7 @@
         <v>238</v>
       </c>
       <c r="W30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X30">
         <v>1500</v>
@@ -5427,7 +5427,7 @@
         <v>86</v>
       </c>
       <c r="AE30" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF30" t="s">
         <v>74</v>
@@ -5442,7 +5442,7 @@
         <v>1970</v>
       </c>
       <c r="AL30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AM30" t="s">
         <v>56</v>
@@ -5454,16 +5454,16 @@
         <v>79</v>
       </c>
       <c r="AP30" t="s">
+        <v>261</v>
+      </c>
+      <c r="AQ30" t="s">
         <v>262</v>
       </c>
-      <c r="AQ30" t="s">
+      <c r="AR30" t="s">
         <v>263</v>
       </c>
-      <c r="AR30" t="s">
+      <c r="AS30" t="s">
         <v>264</v>
-      </c>
-      <c r="AS30" t="s">
-        <v>265</v>
       </c>
       <c r="AU30" t="s">
         <v>57</v>
@@ -5474,7 +5474,7 @@
     </row>
     <row r="31" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B31" t="s">
         <v>50</v>
@@ -5498,7 +5498,7 @@
         <v>49</v>
       </c>
       <c r="I31" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J31" t="s">
         <v>220</v>
@@ -5516,7 +5516,7 @@
         <v>69</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P31" t="s">
         <v>53</v>
@@ -5537,7 +5537,7 @@
         <v>238</v>
       </c>
       <c r="W31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z31">
         <v>6.2676445999999997</v>
@@ -5555,7 +5555,7 @@
         <v>86</v>
       </c>
       <c r="AE31" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF31" t="s">
         <v>74</v>
@@ -5564,13 +5564,13 @@
         <v>190</v>
       </c>
       <c r="AI31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="AJ31">
         <v>2008</v>
       </c>
       <c r="AL31" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AM31" t="s">
         <v>56</v>
@@ -5582,27 +5582,27 @@
         <v>79</v>
       </c>
       <c r="AP31" t="s">
+        <v>269</v>
+      </c>
+      <c r="AQ31" t="s">
         <v>270</v>
       </c>
-      <c r="AQ31" t="s">
+      <c r="AR31" t="s">
         <v>271</v>
       </c>
-      <c r="AR31" t="s">
+      <c r="AS31" t="s">
         <v>272</v>
-      </c>
-      <c r="AS31" t="s">
-        <v>273</v>
       </c>
       <c r="AU31" t="s">
         <v>57</v>
       </c>
       <c r="AV31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B32" t="s">
         <v>50</v>
@@ -5626,7 +5626,7 @@
         <v>49</v>
       </c>
       <c r="I32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J32" t="s">
         <v>220</v>
@@ -5644,7 +5644,7 @@
         <v>69</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P32" t="s">
         <v>53</v>
@@ -5683,7 +5683,7 @@
         <v>86</v>
       </c>
       <c r="AE32" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF32" t="s">
         <v>74</v>
@@ -5698,7 +5698,7 @@
         <v>32937</v>
       </c>
       <c r="AL32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AM32" t="s">
         <v>56</v>
@@ -5716,21 +5716,21 @@
         <v>242</v>
       </c>
       <c r="AR32" t="s">
+        <v>276</v>
+      </c>
+      <c r="AS32" t="s">
         <v>277</v>
-      </c>
-      <c r="AS32" t="s">
-        <v>278</v>
       </c>
       <c r="AU32" t="s">
         <v>57</v>
       </c>
       <c r="AV32" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B33" t="s">
         <v>50</v>
@@ -5754,7 +5754,7 @@
         <v>49</v>
       </c>
       <c r="I33" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J33" t="s">
         <v>220</v>
@@ -5772,7 +5772,7 @@
         <v>69</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P33" t="s">
         <v>53</v>
@@ -5793,7 +5793,7 @@
         <v>238</v>
       </c>
       <c r="W33" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Z33">
         <v>6.2676445999999997</v>
@@ -5811,7 +5811,7 @@
         <v>86</v>
       </c>
       <c r="AE33" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF33" t="s">
         <v>74</v>
@@ -5820,7 +5820,7 @@
         <v>190</v>
       </c>
       <c r="AL33" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AM33" t="s">
         <v>56</v>
@@ -5832,16 +5832,16 @@
         <v>79</v>
       </c>
       <c r="AP33" t="s">
+        <v>281</v>
+      </c>
+      <c r="AQ33" t="s">
         <v>282</v>
       </c>
-      <c r="AQ33" t="s">
+      <c r="AR33" t="s">
         <v>283</v>
       </c>
-      <c r="AR33" t="s">
+      <c r="AS33" t="s">
         <v>284</v>
-      </c>
-      <c r="AS33" t="s">
-        <v>285</v>
       </c>
       <c r="AU33" t="s">
         <v>57</v>
@@ -5849,7 +5849,7 @@
     </row>
     <row r="34" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B34" t="s">
         <v>50</v>
@@ -5873,7 +5873,7 @@
         <v>49</v>
       </c>
       <c r="I34" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J34" t="s">
         <v>220</v>
@@ -5891,7 +5891,7 @@
         <v>69</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P34" t="s">
         <v>53</v>
@@ -5912,7 +5912,7 @@
         <v>222</v>
       </c>
       <c r="W34" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="Z34">
         <v>6.4657999999999998</v>
@@ -5930,7 +5930,7 @@
         <v>224</v>
       </c>
       <c r="AE34" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AF34" t="s">
         <v>74</v>
@@ -5945,7 +5945,7 @@
         <v>1970</v>
       </c>
       <c r="AL34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AM34" t="s">
         <v>56</v>
@@ -5960,24 +5960,24 @@
         <v>88</v>
       </c>
       <c r="AQ34" t="s">
+        <v>288</v>
+      </c>
+      <c r="AR34" t="s">
         <v>289</v>
       </c>
-      <c r="AR34" t="s">
+      <c r="AS34" t="s">
         <v>290</v>
-      </c>
-      <c r="AS34" t="s">
-        <v>291</v>
       </c>
       <c r="AU34" t="s">
         <v>57</v>
       </c>
       <c r="AV34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B35" t="s">
         <v>50</v>
@@ -6001,7 +6001,7 @@
         <v>49</v>
       </c>
       <c r="I35" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J35" t="s">
         <v>220</v>
@@ -6010,7 +6010,7 @@
         <v>1</v>
       </c>
       <c r="L35" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M35" t="s">
         <v>52</v>
@@ -6019,7 +6019,7 @@
         <v>69</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P35" t="s">
         <v>53</v>
@@ -6040,7 +6040,7 @@
         <v>238</v>
       </c>
       <c r="W35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Z35">
         <v>6.2676445999999997</v>
@@ -6058,7 +6058,7 @@
         <v>86</v>
       </c>
       <c r="AE35" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF35" t="s">
         <v>74</v>
@@ -6067,10 +6067,10 @@
         <v>190</v>
       </c>
       <c r="AI35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AL35" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AM35" t="s">
         <v>56</v>
@@ -6082,16 +6082,16 @@
         <v>79</v>
       </c>
       <c r="AP35" t="s">
+        <v>281</v>
+      </c>
+      <c r="AQ35" t="s">
         <v>282</v>
       </c>
-      <c r="AQ35" t="s">
-        <v>283</v>
-      </c>
       <c r="AR35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AS35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AU35" t="s">
         <v>57</v>

</xml_diff>